<commit_message>
202108150409 - Update View, ProcessController, result
</commit_message>
<xml_diff>
--- a/result/Mau test 12.xlsx
+++ b/result/Mau test 12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvmin\workspace\ColorMixing-Java\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC095BDF-8CF3-446D-90ED-8166064B3F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA26EA2-4A45-460E-AE41-20454BCFABFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample data" sheetId="1" r:id="rId1"/>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS16418"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AS1"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55661,8 +55661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55882,26 +55882,66 @@
       <c r="Y2" s="5">
         <v>54.59</v>
       </c>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
+      <c r="Z2" s="5">
+        <v>55.77</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>56.69</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>61.46</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>6.18</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>3.75</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="5">
+        <v>29.91</v>
+      </c>
+      <c r="AP2" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="AQ2" s="5">
+        <v>13.92</v>
+      </c>
+      <c r="AR2" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="AS2" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -55979,26 +56019,66 @@
       <c r="Y3" s="5">
         <v>0</v>
       </c>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="5"/>
-      <c r="AO3" s="5"/>
-      <c r="AP3" s="5"/>
-      <c r="AQ3" s="5"/>
-      <c r="AR3" s="5"/>
-      <c r="AS3" s="5"/>
+      <c r="Z3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>3.75</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -56076,26 +56156,66 @@
       <c r="Y4" s="5">
         <v>45.41</v>
       </c>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AM4" s="5"/>
-      <c r="AN4" s="5"/>
-      <c r="AO4" s="5"/>
-      <c r="AP4" s="5"/>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="5"/>
-      <c r="AS4" s="5"/>
+      <c r="Z4" s="5">
+        <v>44.23</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>43.31</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>38.54</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>8.93</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>5.58</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>9</v>
+      </c>
+      <c r="AN4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>41.92</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>31.26</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>28.8</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>3.68</v>
+      </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -56173,26 +56293,66 @@
       <c r="Y5" s="5">
         <v>0</v>
       </c>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="5"/>
-      <c r="AO5" s="5"/>
-      <c r="AP5" s="5"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
+      <c r="Z5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>99.58</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>100</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>99.98</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>98.84</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>98.1</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>100</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>84.89</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>90.67</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>99.56</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>99.42</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>83.19</v>
+      </c>
+      <c r="AN5" s="5">
+        <v>96.25</v>
+      </c>
+      <c r="AO5" s="5">
+        <v>28.17</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>50.44</v>
+      </c>
+      <c r="AQ5" s="5">
+        <v>57.28</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>99.2</v>
+      </c>
+      <c r="AS5" s="5">
+        <v>96.32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>